<commit_message>
modify excel files and figures
</commit_message>
<xml_diff>
--- a/excel_files/fadScores.xlsx
+++ b/excel_files/fadScores.xlsx
@@ -25,6 +25,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="wavlm-base-plus" sheetId="16" state="visible" r:id="rId16"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="wavlm-base" sheetId="17" state="visible" r:id="rId17"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="wavlm-large" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="joint-scat" sheetId="19" state="visible" r:id="rId19"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3886,6 +3887,351 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>alg_code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dog_bark</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>footstep</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>gunshot</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>keyboard</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>moving_motor_vehicle</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>rain</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sneeze_cough</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>avg_category_FAD</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>Baseline</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>6412.108822858143</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16177.61467798351</v>
+      </c>
+      <c r="D2" t="n">
+        <v>226877.2591667986</v>
+      </c>
+      <c r="E2" t="n">
+        <v>39450.46834742428</v>
+      </c>
+      <c r="F2" t="n">
+        <v>417760.8205551166</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1246.460676927177</v>
+      </c>
+      <c r="H2" t="n">
+        <v>58884.08675310281</v>
+      </c>
+      <c r="I2" t="n">
+        <v>109544.1170000301</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>TASys02</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>2164.677705544587</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11466.7227572848</v>
+      </c>
+      <c r="D3" t="n">
+        <v>12766.89027288463</v>
+      </c>
+      <c r="E3" t="n">
+        <v>120962.860210016</v>
+      </c>
+      <c r="F3" t="n">
+        <v>345588.3932784392</v>
+      </c>
+      <c r="G3" t="n">
+        <v>9572.154394896079</v>
+      </c>
+      <c r="H3" t="n">
+        <v>34048.72736894032</v>
+      </c>
+      <c r="I3" t="n">
+        <v>76652.91799828652</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>TASys03</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>8326.955484781982</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7925.430432487436</v>
+      </c>
+      <c r="D4" t="n">
+        <v>228332.4501374071</v>
+      </c>
+      <c r="E4" t="n">
+        <v>127955.5979676959</v>
+      </c>
+      <c r="F4" t="n">
+        <v>795967.2159420585</v>
+      </c>
+      <c r="G4" t="n">
+        <v>9027.467967408056</v>
+      </c>
+      <c r="H4" t="n">
+        <v>101063.4592286405</v>
+      </c>
+      <c r="I4" t="n">
+        <v>182656.9395943542</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>TASys08</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>5475.915396630806</v>
+      </c>
+      <c r="C5" t="n">
+        <v>3494.91337050969</v>
+      </c>
+      <c r="D5" t="n">
+        <v>165748.3614948218</v>
+      </c>
+      <c r="E5" t="n">
+        <v>111226.6460575687</v>
+      </c>
+      <c r="F5" t="n">
+        <v>831672.3790306748</v>
+      </c>
+      <c r="G5" t="n">
+        <v>7507.48932138861</v>
+      </c>
+      <c r="H5" t="n">
+        <v>101363.203904979</v>
+      </c>
+      <c r="I5" t="n">
+        <v>175212.7012252247</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>TASys11</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>7599.925545613903</v>
+      </c>
+      <c r="C6" t="n">
+        <v>150297.0603118276</v>
+      </c>
+      <c r="D6" t="n">
+        <v>297024.9416328784</v>
+      </c>
+      <c r="E6" t="n">
+        <v>24044.90400988286</v>
+      </c>
+      <c r="F6" t="n">
+        <v>837198.6016055684</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8100.835438509881</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4753.224838072987</v>
+      </c>
+      <c r="I6" t="n">
+        <v>189859.9276260506</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>TBSys09</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4490.060552633944</v>
+      </c>
+      <c r="C7" t="n">
+        <v>7256.478243895912</v>
+      </c>
+      <c r="D7" t="n">
+        <v>154775210.6032548</v>
+      </c>
+      <c r="E7" t="n">
+        <v>94578.96995438276</v>
+      </c>
+      <c r="F7" t="n">
+        <v>572297.5011757913</v>
+      </c>
+      <c r="G7" t="n">
+        <v>197.2951573284226</v>
+      </c>
+      <c r="H7" t="n">
+        <v>95317.25800536814</v>
+      </c>
+      <c r="I7" t="n">
+        <v>22221335.45233488</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>TBSys14</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>5868.400010851554</v>
+      </c>
+      <c r="C8" t="n">
+        <v>255.1290328809373</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3120145.402389309</v>
+      </c>
+      <c r="E8" t="n">
+        <v>105883.8738016963</v>
+      </c>
+      <c r="F8" t="n">
+        <v>761575.5037789284</v>
+      </c>
+      <c r="G8" t="n">
+        <v>2405.658471966781</v>
+      </c>
+      <c r="H8" t="n">
+        <v>66856.95550418066</v>
+      </c>
+      <c r="I8" t="n">
+        <v>580427.2747128305</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>TBSys18</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>956.6505526141482</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1110.401407768937</v>
+      </c>
+      <c r="D9" t="n">
+        <v>270358.8138694638</v>
+      </c>
+      <c r="E9" t="n">
+        <v>108498.1348472907</v>
+      </c>
+      <c r="F9" t="n">
+        <v>812192.4827031174</v>
+      </c>
+      <c r="G9" t="n">
+        <v>928.9746406285522</v>
+      </c>
+      <c r="H9" t="n">
+        <v>88940.92322370921</v>
+      </c>
+      <c r="I9" t="n">
+        <v>183283.7687492275</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>TBSys24</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3290.537615515859</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2559.433608909461</v>
+      </c>
+      <c r="D10" t="n">
+        <v>129508.1255027545</v>
+      </c>
+      <c r="E10" t="n">
+        <v>100784.188118854</v>
+      </c>
+      <c r="F10" t="n">
+        <v>701252.0431087858</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2720.61437615156</v>
+      </c>
+      <c r="H10" t="n">
+        <v>59086.40307576059</v>
+      </c>
+      <c r="I10" t="n">
+        <v>142743.0493438188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>

</xml_diff>